<commit_message>
updated changes - 2022-07-02 11:44:26
</commit_message>
<xml_diff>
--- a/app/src/test/resources/Dataset.xlsx
+++ b/app/src/test/resources/Dataset.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="38">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -79,37 +79,28 @@
     <t>[Connector, Kindle]</t>
   </si>
   <si>
+    <t>TestCase07</t>
+  </si>
+  <si>
+    <t>[Tan Leatherette Weekender Duffle;Xtend Smart Watch]</t>
+  </si>
+  <si>
+    <t>[Connector;Xtend Smart Watch]</t>
+  </si>
+  <si>
+    <t>[Kindle;Jenga]</t>
+  </si>
+  <si>
     <t>TestCase08</t>
   </si>
   <si>
-    <t>[Tan Leatherette Weekender Duffle;Xtend Smart Watch]</t>
-  </si>
-  <si>
-    <t>TestCase07</t>
-  </si>
-  <si>
-    <t>[Connector;Xtend Smart Watch]</t>
-  </si>
-  <si>
-    <t>TestCase09</t>
-  </si>
-  <si>
-    <t>[Kindle;Jenga]</t>
-  </si>
-  <si>
     <t>[Tan Leatherette Weekender Duffle, 60.0]</t>
   </si>
   <si>
     <t>[SuitCase, 50.0]</t>
   </si>
   <si>
-    <t>TestCase10</t>
-  </si>
-  <si>
     <t>[Jenga, 60.0]</t>
-  </si>
-  <si>
-    <t>[]</t>
   </si>
   <si>
     <t>TestCase11</t>
@@ -549,7 +540,7 @@
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -558,42 +549,42 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="1" t="s">
+    </row>
+    <row r="22" ht="15.75" customHeight="1">
+      <c r="A22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="1" t="s">
+    <row r="23" ht="15.75" customHeight="1">
+      <c r="A23" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="1" t="s">
+    <row r="24" ht="15.75" customHeight="1">
+      <c r="A24" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="1" t="s">
+    <row r="25" ht="15.75" customHeight="1">
+      <c r="A25" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
@@ -601,11 +592,11 @@
         <v>30</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -613,16 +604,16 @@
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>35</v>
@@ -630,7 +621,7 @@
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>36</v>
@@ -638,28 +629,14 @@
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
+    </row>
+    <row r="32" ht="15.75" customHeight="1"/>
+    <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>
     <row r="36" ht="15.75" customHeight="1"/>
@@ -1624,8 +1601,6 @@
     <row r="995" ht="15.75" customHeight="1"/>
     <row r="996" ht="15.75" customHeight="1"/>
     <row r="997" ht="15.75" customHeight="1"/>
-    <row r="998" ht="15.75" customHeight="1"/>
-    <row r="999" ht="15.75" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
updated changes - 2022-07-02 11:44:30
</commit_message>
<xml_diff>
--- a/app/src/test/resources/Dataset.xlsx
+++ b/app/src/test/resources/Dataset.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="38">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -79,37 +79,28 @@
     <t>[Connector, Kindle]</t>
   </si>
   <si>
+    <t>TestCase07</t>
+  </si>
+  <si>
+    <t>[Tan Leatherette Weekender Duffle;Xtend Smart Watch]</t>
+  </si>
+  <si>
+    <t>[Connector;Xtend Smart Watch]</t>
+  </si>
+  <si>
+    <t>[Kindle;Jenga]</t>
+  </si>
+  <si>
     <t>TestCase08</t>
   </si>
   <si>
-    <t>[Tan Leatherette Weekender Duffle;Xtend Smart Watch]</t>
-  </si>
-  <si>
-    <t>TestCase07</t>
-  </si>
-  <si>
-    <t>[Connector;Xtend Smart Watch]</t>
-  </si>
-  <si>
-    <t>TestCase09</t>
-  </si>
-  <si>
-    <t>[Kindle;Jenga]</t>
-  </si>
-  <si>
     <t>[Tan Leatherette Weekender Duffle, 60.0]</t>
   </si>
   <si>
     <t>[SuitCase, 50.0]</t>
   </si>
   <si>
-    <t>TestCase10</t>
-  </si>
-  <si>
     <t>[Jenga, 60.0]</t>
-  </si>
-  <si>
-    <t>[]</t>
   </si>
   <si>
     <t>TestCase11</t>
@@ -549,7 +540,7 @@
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -558,42 +549,42 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="1" t="s">
+    </row>
+    <row r="22" ht="15.75" customHeight="1">
+      <c r="A22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="1" t="s">
+    <row r="23" ht="15.75" customHeight="1">
+      <c r="A23" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="1" t="s">
+    <row r="24" ht="15.75" customHeight="1">
+      <c r="A24" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="1" t="s">
+    <row r="25" ht="15.75" customHeight="1">
+      <c r="A25" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
@@ -601,11 +592,11 @@
         <v>30</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -613,16 +604,16 @@
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>35</v>
@@ -630,7 +621,7 @@
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>36</v>
@@ -638,28 +629,14 @@
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
+    </row>
+    <row r="32" ht="15.75" customHeight="1"/>
+    <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>
     <row r="36" ht="15.75" customHeight="1"/>
@@ -1624,8 +1601,6 @@
     <row r="995" ht="15.75" customHeight="1"/>
     <row r="996" ht="15.75" customHeight="1"/>
     <row r="997" ht="15.75" customHeight="1"/>
-    <row r="998" ht="15.75" customHeight="1"/>
-    <row r="999" ht="15.75" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
updated changes - 2022-07-02 11:44:33
</commit_message>
<xml_diff>
--- a/app/src/test/resources/Dataset.xlsx
+++ b/app/src/test/resources/Dataset.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="38">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -79,37 +79,28 @@
     <t>[Connector, Kindle]</t>
   </si>
   <si>
+    <t>TestCase07</t>
+  </si>
+  <si>
+    <t>[Tan Leatherette Weekender Duffle;Xtend Smart Watch]</t>
+  </si>
+  <si>
+    <t>[Connector;Xtend Smart Watch]</t>
+  </si>
+  <si>
+    <t>[Kindle;Jenga]</t>
+  </si>
+  <si>
     <t>TestCase08</t>
   </si>
   <si>
-    <t>[Tan Leatherette Weekender Duffle;Xtend Smart Watch]</t>
-  </si>
-  <si>
-    <t>TestCase07</t>
-  </si>
-  <si>
-    <t>[Connector;Xtend Smart Watch]</t>
-  </si>
-  <si>
-    <t>TestCase09</t>
-  </si>
-  <si>
-    <t>[Kindle;Jenga]</t>
-  </si>
-  <si>
     <t>[Tan Leatherette Weekender Duffle, 60.0]</t>
   </si>
   <si>
     <t>[SuitCase, 50.0]</t>
   </si>
   <si>
-    <t>TestCase10</t>
-  </si>
-  <si>
     <t>[Jenga, 60.0]</t>
-  </si>
-  <si>
-    <t>[]</t>
   </si>
   <si>
     <t>TestCase11</t>
@@ -549,7 +540,7 @@
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -558,42 +549,42 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="1" t="s">
+    </row>
+    <row r="22" ht="15.75" customHeight="1">
+      <c r="A22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="1" t="s">
+    <row r="23" ht="15.75" customHeight="1">
+      <c r="A23" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="1" t="s">
+    <row r="24" ht="15.75" customHeight="1">
+      <c r="A24" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="1" t="s">
+    <row r="25" ht="15.75" customHeight="1">
+      <c r="A25" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
@@ -601,11 +592,11 @@
         <v>30</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -613,16 +604,16 @@
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>35</v>
@@ -630,7 +621,7 @@
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>36</v>
@@ -638,28 +629,14 @@
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
+    </row>
+    <row r="32" ht="15.75" customHeight="1"/>
+    <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>
     <row r="36" ht="15.75" customHeight="1"/>
@@ -1624,8 +1601,6 @@
     <row r="995" ht="15.75" customHeight="1"/>
     <row r="996" ht="15.75" customHeight="1"/>
     <row r="997" ht="15.75" customHeight="1"/>
-    <row r="998" ht="15.75" customHeight="1"/>
-    <row r="999" ht="15.75" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
updated changes - 2022-07-02 11:44:36
</commit_message>
<xml_diff>
--- a/app/src/test/resources/Dataset.xlsx
+++ b/app/src/test/resources/Dataset.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="38">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -79,37 +79,28 @@
     <t>[Connector, Kindle]</t>
   </si>
   <si>
+    <t>TestCase07</t>
+  </si>
+  <si>
+    <t>[Tan Leatherette Weekender Duffle;Xtend Smart Watch]</t>
+  </si>
+  <si>
+    <t>[Connector;Xtend Smart Watch]</t>
+  </si>
+  <si>
+    <t>[Kindle;Jenga]</t>
+  </si>
+  <si>
     <t>TestCase08</t>
   </si>
   <si>
-    <t>[Tan Leatherette Weekender Duffle;Xtend Smart Watch]</t>
-  </si>
-  <si>
-    <t>TestCase07</t>
-  </si>
-  <si>
-    <t>[Connector;Xtend Smart Watch]</t>
-  </si>
-  <si>
-    <t>TestCase09</t>
-  </si>
-  <si>
-    <t>[Kindle;Jenga]</t>
-  </si>
-  <si>
     <t>[Tan Leatherette Weekender Duffle, 60.0]</t>
   </si>
   <si>
     <t>[SuitCase, 50.0]</t>
   </si>
   <si>
-    <t>TestCase10</t>
-  </si>
-  <si>
     <t>[Jenga, 60.0]</t>
-  </si>
-  <si>
-    <t>[]</t>
   </si>
   <si>
     <t>TestCase11</t>
@@ -549,7 +540,7 @@
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -558,42 +549,42 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="1" t="s">
+    </row>
+    <row r="22" ht="15.75" customHeight="1">
+      <c r="A22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="1" t="s">
+    <row r="23" ht="15.75" customHeight="1">
+      <c r="A23" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="1" t="s">
+    <row r="24" ht="15.75" customHeight="1">
+      <c r="A24" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="1" t="s">
+    <row r="25" ht="15.75" customHeight="1">
+      <c r="A25" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
@@ -601,11 +592,11 @@
         <v>30</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -613,16 +604,16 @@
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>35</v>
@@ -630,7 +621,7 @@
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>36</v>
@@ -638,28 +629,14 @@
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
+    </row>
+    <row r="32" ht="15.75" customHeight="1"/>
+    <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>
     <row r="36" ht="15.75" customHeight="1"/>
@@ -1624,8 +1601,6 @@
     <row r="995" ht="15.75" customHeight="1"/>
     <row r="996" ht="15.75" customHeight="1"/>
     <row r="997" ht="15.75" customHeight="1"/>
-    <row r="998" ht="15.75" customHeight="1"/>
-    <row r="999" ht="15.75" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
updated changes - 2022-07-02 11:44:40
</commit_message>
<xml_diff>
--- a/app/src/test/resources/Dataset.xlsx
+++ b/app/src/test/resources/Dataset.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="38">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -79,37 +79,28 @@
     <t>[Connector, Kindle]</t>
   </si>
   <si>
+    <t>TestCase07</t>
+  </si>
+  <si>
+    <t>[Tan Leatherette Weekender Duffle;Xtend Smart Watch]</t>
+  </si>
+  <si>
+    <t>[Connector;Xtend Smart Watch]</t>
+  </si>
+  <si>
+    <t>[Kindle;Jenga]</t>
+  </si>
+  <si>
     <t>TestCase08</t>
   </si>
   <si>
-    <t>[Tan Leatherette Weekender Duffle;Xtend Smart Watch]</t>
-  </si>
-  <si>
-    <t>TestCase07</t>
-  </si>
-  <si>
-    <t>[Connector;Xtend Smart Watch]</t>
-  </si>
-  <si>
-    <t>TestCase09</t>
-  </si>
-  <si>
-    <t>[Kindle;Jenga]</t>
-  </si>
-  <si>
     <t>[Tan Leatherette Weekender Duffle, 60.0]</t>
   </si>
   <si>
     <t>[SuitCase, 50.0]</t>
   </si>
   <si>
-    <t>TestCase10</t>
-  </si>
-  <si>
     <t>[Jenga, 60.0]</t>
-  </si>
-  <si>
-    <t>[]</t>
   </si>
   <si>
     <t>TestCase11</t>
@@ -549,7 +540,7 @@
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -558,42 +549,42 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="1" t="s">
+    </row>
+    <row r="22" ht="15.75" customHeight="1">
+      <c r="A22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="1" t="s">
+    <row r="23" ht="15.75" customHeight="1">
+      <c r="A23" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="1" t="s">
+    <row r="24" ht="15.75" customHeight="1">
+      <c r="A24" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="1" t="s">
+    <row r="25" ht="15.75" customHeight="1">
+      <c r="A25" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
@@ -601,11 +592,11 @@
         <v>30</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -613,16 +604,16 @@
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>35</v>
@@ -630,7 +621,7 @@
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>36</v>
@@ -638,28 +629,14 @@
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
+    </row>
+    <row r="32" ht="15.75" customHeight="1"/>
+    <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>
     <row r="36" ht="15.75" customHeight="1"/>
@@ -1624,8 +1601,6 @@
     <row r="995" ht="15.75" customHeight="1"/>
     <row r="996" ht="15.75" customHeight="1"/>
     <row r="997" ht="15.75" customHeight="1"/>
-    <row r="998" ht="15.75" customHeight="1"/>
-    <row r="999" ht="15.75" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
updated changes - 2022-07-04 19:15:53
</commit_message>
<xml_diff>
--- a/app/src/test/resources/Dataset.xlsx
+++ b/app/src/test/resources/Dataset.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="55">
   <si>
     <t>#</t>
   </si>
@@ -55,40 +55,46 @@
     <t>YONEX</t>
   </si>
   <si>
+    <t>ROADSTER</t>
+  </si>
+  <si>
+    <t>CONNECTOR</t>
+  </si>
+  <si>
+    <t>TC4_ProductNameToSearchFor</t>
+  </si>
+  <si>
+    <t>Nike Mens Running Shoes</t>
+  </si>
+  <si>
     <t>Roadster</t>
   </si>
   <si>
+    <t>HandBag</t>
+  </si>
+  <si>
+    <t>TC5_ProductNameToSearchFor</t>
+  </si>
+  <si>
+    <t>TC5_ProductNameToSearchFor2</t>
+  </si>
+  <si>
+    <t>TC5_AddressDetails</t>
+  </si>
+  <si>
+    <t>YONEX Smash Badminton Racquet</t>
+  </si>
+  <si>
+    <t>Tan Leatherette Weekender Duffle</t>
+  </si>
+  <si>
+    <t>Addr line 1 addr Line 2 addr line 3</t>
+  </si>
+  <si>
+    <t>TEST ADDR LINES COUNT GREATER TH</t>
+  </si>
+  <si>
     <t>Connector</t>
-  </si>
-  <si>
-    <t>TC4_ProductNameToSearchFor</t>
-  </si>
-  <si>
-    <t>Nike Mens Running Shoes</t>
-  </si>
-  <si>
-    <t>HandBag</t>
-  </si>
-  <si>
-    <t>TC5_ProductNameToSearchFor</t>
-  </si>
-  <si>
-    <t>TC5_ProductNameToSearchFor2</t>
-  </si>
-  <si>
-    <t>TC5_AddressDetails</t>
-  </si>
-  <si>
-    <t>YONEX Smash Badminton Racquet</t>
-  </si>
-  <si>
-    <t>Tan Leatherette Weekender Duffle</t>
-  </si>
-  <si>
-    <t>Addr line 1 addr Line 2 addr line 3</t>
-  </si>
-  <si>
-    <t>TEST ADDR LINES COUNT GREATER TH</t>
   </si>
   <si>
     <t>1 Hacker Way Menlo Park, CA 94025</t>
@@ -642,10 +648,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2">
@@ -653,10 +659,10 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3">
@@ -664,10 +670,10 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4">
@@ -675,10 +681,10 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -832,7 +838,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4">
@@ -840,7 +846,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5">
@@ -3855,13 +3861,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2">
@@ -3869,13 +3875,13 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3">
@@ -3883,13 +3889,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4">
@@ -3897,13 +3903,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -3930,10 +3936,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2">
@@ -3941,10 +3947,10 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3">
@@ -3952,10 +3958,10 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4">
@@ -3963,10 +3969,10 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -3992,7 +3998,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2">
@@ -4000,7 +4006,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3">
@@ -4008,7 +4014,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4">
@@ -4016,7 +4022,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -4042,10 +4048,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2">
@@ -4053,7 +4059,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C2" s="7">
         <v>60.0</v>
@@ -4064,7 +4070,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C3" s="7">
         <v>50.0</v>
@@ -4075,7 +4081,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C4" s="7">
         <v>60.0</v>
@@ -4106,13 +4112,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2">
@@ -4120,13 +4126,13 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3">
@@ -4134,13 +4140,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4">
@@ -4148,13 +4154,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
updated changes - 2022-07-04 19:15:57
</commit_message>
<xml_diff>
--- a/app/src/test/resources/Dataset.xlsx
+++ b/app/src/test/resources/Dataset.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="55">
   <si>
     <t>#</t>
   </si>
@@ -55,40 +55,46 @@
     <t>YONEX</t>
   </si>
   <si>
+    <t>ROADSTER</t>
+  </si>
+  <si>
+    <t>CONNECTOR</t>
+  </si>
+  <si>
+    <t>TC4_ProductNameToSearchFor</t>
+  </si>
+  <si>
+    <t>Nike Mens Running Shoes</t>
+  </si>
+  <si>
     <t>Roadster</t>
   </si>
   <si>
+    <t>HandBag</t>
+  </si>
+  <si>
+    <t>TC5_ProductNameToSearchFor</t>
+  </si>
+  <si>
+    <t>TC5_ProductNameToSearchFor2</t>
+  </si>
+  <si>
+    <t>TC5_AddressDetails</t>
+  </si>
+  <si>
+    <t>YONEX Smash Badminton Racquet</t>
+  </si>
+  <si>
+    <t>Tan Leatherette Weekender Duffle</t>
+  </si>
+  <si>
+    <t>Addr line 1 addr Line 2 addr line 3</t>
+  </si>
+  <si>
+    <t>TEST ADDR LINES COUNT GREATER TH</t>
+  </si>
+  <si>
     <t>Connector</t>
-  </si>
-  <si>
-    <t>TC4_ProductNameToSearchFor</t>
-  </si>
-  <si>
-    <t>Nike Mens Running Shoes</t>
-  </si>
-  <si>
-    <t>HandBag</t>
-  </si>
-  <si>
-    <t>TC5_ProductNameToSearchFor</t>
-  </si>
-  <si>
-    <t>TC5_ProductNameToSearchFor2</t>
-  </si>
-  <si>
-    <t>TC5_AddressDetails</t>
-  </si>
-  <si>
-    <t>YONEX Smash Badminton Racquet</t>
-  </si>
-  <si>
-    <t>Tan Leatherette Weekender Duffle</t>
-  </si>
-  <si>
-    <t>Addr line 1 addr Line 2 addr line 3</t>
-  </si>
-  <si>
-    <t>TEST ADDR LINES COUNT GREATER TH</t>
   </si>
   <si>
     <t>1 Hacker Way Menlo Park, CA 94025</t>
@@ -642,10 +648,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2">
@@ -653,10 +659,10 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3">
@@ -664,10 +670,10 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4">
@@ -675,10 +681,10 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -832,7 +838,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4">
@@ -840,7 +846,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5">
@@ -3855,13 +3861,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2">
@@ -3869,13 +3875,13 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3">
@@ -3883,13 +3889,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4">
@@ -3897,13 +3903,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -3930,10 +3936,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2">
@@ -3941,10 +3947,10 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3">
@@ -3952,10 +3958,10 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4">
@@ -3963,10 +3969,10 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -3992,7 +3998,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2">
@@ -4000,7 +4006,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3">
@@ -4008,7 +4014,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4">
@@ -4016,7 +4022,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -4042,10 +4048,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2">
@@ -4053,7 +4059,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C2" s="7">
         <v>60.0</v>
@@ -4064,7 +4070,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C3" s="7">
         <v>50.0</v>
@@ -4075,7 +4081,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C4" s="7">
         <v>60.0</v>
@@ -4106,13 +4112,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2">
@@ -4120,13 +4126,13 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3">
@@ -4134,13 +4140,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4">
@@ -4148,13 +4154,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
updated changes - 2022-07-04 19:15:59
</commit_message>
<xml_diff>
--- a/app/src/test/resources/Dataset.xlsx
+++ b/app/src/test/resources/Dataset.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="55">
   <si>
     <t>#</t>
   </si>
@@ -55,40 +55,46 @@
     <t>YONEX</t>
   </si>
   <si>
+    <t>ROADSTER</t>
+  </si>
+  <si>
+    <t>CONNECTOR</t>
+  </si>
+  <si>
+    <t>TC4_ProductNameToSearchFor</t>
+  </si>
+  <si>
+    <t>Nike Mens Running Shoes</t>
+  </si>
+  <si>
     <t>Roadster</t>
   </si>
   <si>
+    <t>HandBag</t>
+  </si>
+  <si>
+    <t>TC5_ProductNameToSearchFor</t>
+  </si>
+  <si>
+    <t>TC5_ProductNameToSearchFor2</t>
+  </si>
+  <si>
+    <t>TC5_AddressDetails</t>
+  </si>
+  <si>
+    <t>YONEX Smash Badminton Racquet</t>
+  </si>
+  <si>
+    <t>Tan Leatherette Weekender Duffle</t>
+  </si>
+  <si>
+    <t>Addr line 1 addr Line 2 addr line 3</t>
+  </si>
+  <si>
+    <t>TEST ADDR LINES COUNT GREATER TH</t>
+  </si>
+  <si>
     <t>Connector</t>
-  </si>
-  <si>
-    <t>TC4_ProductNameToSearchFor</t>
-  </si>
-  <si>
-    <t>Nike Mens Running Shoes</t>
-  </si>
-  <si>
-    <t>HandBag</t>
-  </si>
-  <si>
-    <t>TC5_ProductNameToSearchFor</t>
-  </si>
-  <si>
-    <t>TC5_ProductNameToSearchFor2</t>
-  </si>
-  <si>
-    <t>TC5_AddressDetails</t>
-  </si>
-  <si>
-    <t>YONEX Smash Badminton Racquet</t>
-  </si>
-  <si>
-    <t>Tan Leatherette Weekender Duffle</t>
-  </si>
-  <si>
-    <t>Addr line 1 addr Line 2 addr line 3</t>
-  </si>
-  <si>
-    <t>TEST ADDR LINES COUNT GREATER TH</t>
   </si>
   <si>
     <t>1 Hacker Way Menlo Park, CA 94025</t>
@@ -642,10 +648,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2">
@@ -653,10 +659,10 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3">
@@ -664,10 +670,10 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4">
@@ -675,10 +681,10 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -832,7 +838,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4">
@@ -840,7 +846,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5">
@@ -3855,13 +3861,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2">
@@ -3869,13 +3875,13 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3">
@@ -3883,13 +3889,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4">
@@ -3897,13 +3903,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -3930,10 +3936,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2">
@@ -3941,10 +3947,10 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3">
@@ -3952,10 +3958,10 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4">
@@ -3963,10 +3969,10 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -3992,7 +3998,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2">
@@ -4000,7 +4006,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3">
@@ -4008,7 +4014,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4">
@@ -4016,7 +4022,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -4042,10 +4048,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2">
@@ -4053,7 +4059,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C2" s="7">
         <v>60.0</v>
@@ -4064,7 +4070,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C3" s="7">
         <v>50.0</v>
@@ -4075,7 +4081,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C4" s="7">
         <v>60.0</v>
@@ -4106,13 +4112,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2">
@@ -4120,13 +4126,13 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3">
@@ -4134,13 +4140,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4">
@@ -4148,13 +4154,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
updated changes - 2022-07-04 19:16:02
</commit_message>
<xml_diff>
--- a/app/src/test/resources/Dataset.xlsx
+++ b/app/src/test/resources/Dataset.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="55">
   <si>
     <t>#</t>
   </si>
@@ -55,40 +55,46 @@
     <t>YONEX</t>
   </si>
   <si>
+    <t>ROADSTER</t>
+  </si>
+  <si>
+    <t>CONNECTOR</t>
+  </si>
+  <si>
+    <t>TC4_ProductNameToSearchFor</t>
+  </si>
+  <si>
+    <t>Nike Mens Running Shoes</t>
+  </si>
+  <si>
     <t>Roadster</t>
   </si>
   <si>
+    <t>HandBag</t>
+  </si>
+  <si>
+    <t>TC5_ProductNameToSearchFor</t>
+  </si>
+  <si>
+    <t>TC5_ProductNameToSearchFor2</t>
+  </si>
+  <si>
+    <t>TC5_AddressDetails</t>
+  </si>
+  <si>
+    <t>YONEX Smash Badminton Racquet</t>
+  </si>
+  <si>
+    <t>Tan Leatherette Weekender Duffle</t>
+  </si>
+  <si>
+    <t>Addr line 1 addr Line 2 addr line 3</t>
+  </si>
+  <si>
+    <t>TEST ADDR LINES COUNT GREATER TH</t>
+  </si>
+  <si>
     <t>Connector</t>
-  </si>
-  <si>
-    <t>TC4_ProductNameToSearchFor</t>
-  </si>
-  <si>
-    <t>Nike Mens Running Shoes</t>
-  </si>
-  <si>
-    <t>HandBag</t>
-  </si>
-  <si>
-    <t>TC5_ProductNameToSearchFor</t>
-  </si>
-  <si>
-    <t>TC5_ProductNameToSearchFor2</t>
-  </si>
-  <si>
-    <t>TC5_AddressDetails</t>
-  </si>
-  <si>
-    <t>YONEX Smash Badminton Racquet</t>
-  </si>
-  <si>
-    <t>Tan Leatherette Weekender Duffle</t>
-  </si>
-  <si>
-    <t>Addr line 1 addr Line 2 addr line 3</t>
-  </si>
-  <si>
-    <t>TEST ADDR LINES COUNT GREATER TH</t>
   </si>
   <si>
     <t>1 Hacker Way Menlo Park, CA 94025</t>
@@ -642,10 +648,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2">
@@ -653,10 +659,10 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3">
@@ -664,10 +670,10 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4">
@@ -675,10 +681,10 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -832,7 +838,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4">
@@ -840,7 +846,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5">
@@ -3855,13 +3861,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2">
@@ -3869,13 +3875,13 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3">
@@ -3883,13 +3889,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4">
@@ -3897,13 +3903,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -3930,10 +3936,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2">
@@ -3941,10 +3947,10 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3">
@@ -3952,10 +3958,10 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4">
@@ -3963,10 +3969,10 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -3992,7 +3998,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2">
@@ -4000,7 +4006,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3">
@@ -4008,7 +4014,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4">
@@ -4016,7 +4022,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -4042,10 +4048,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2">
@@ -4053,7 +4059,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C2" s="7">
         <v>60.0</v>
@@ -4064,7 +4070,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C3" s="7">
         <v>50.0</v>
@@ -4075,7 +4081,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C4" s="7">
         <v>60.0</v>
@@ -4106,13 +4112,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2">
@@ -4120,13 +4126,13 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3">
@@ -4134,13 +4140,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4">
@@ -4148,13 +4154,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
updated changes - 2022-07-04 19:16:06
</commit_message>
<xml_diff>
--- a/app/src/test/resources/Dataset.xlsx
+++ b/app/src/test/resources/Dataset.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="55">
   <si>
     <t>#</t>
   </si>
@@ -55,40 +55,46 @@
     <t>YONEX</t>
   </si>
   <si>
+    <t>ROADSTER</t>
+  </si>
+  <si>
+    <t>CONNECTOR</t>
+  </si>
+  <si>
+    <t>TC4_ProductNameToSearchFor</t>
+  </si>
+  <si>
+    <t>Nike Mens Running Shoes</t>
+  </si>
+  <si>
     <t>Roadster</t>
   </si>
   <si>
+    <t>HandBag</t>
+  </si>
+  <si>
+    <t>TC5_ProductNameToSearchFor</t>
+  </si>
+  <si>
+    <t>TC5_ProductNameToSearchFor2</t>
+  </si>
+  <si>
+    <t>TC5_AddressDetails</t>
+  </si>
+  <si>
+    <t>YONEX Smash Badminton Racquet</t>
+  </si>
+  <si>
+    <t>Tan Leatherette Weekender Duffle</t>
+  </si>
+  <si>
+    <t>Addr line 1 addr Line 2 addr line 3</t>
+  </si>
+  <si>
+    <t>TEST ADDR LINES COUNT GREATER TH</t>
+  </si>
+  <si>
     <t>Connector</t>
-  </si>
-  <si>
-    <t>TC4_ProductNameToSearchFor</t>
-  </si>
-  <si>
-    <t>Nike Mens Running Shoes</t>
-  </si>
-  <si>
-    <t>HandBag</t>
-  </si>
-  <si>
-    <t>TC5_ProductNameToSearchFor</t>
-  </si>
-  <si>
-    <t>TC5_ProductNameToSearchFor2</t>
-  </si>
-  <si>
-    <t>TC5_AddressDetails</t>
-  </si>
-  <si>
-    <t>YONEX Smash Badminton Racquet</t>
-  </si>
-  <si>
-    <t>Tan Leatherette Weekender Duffle</t>
-  </si>
-  <si>
-    <t>Addr line 1 addr Line 2 addr line 3</t>
-  </si>
-  <si>
-    <t>TEST ADDR LINES COUNT GREATER TH</t>
   </si>
   <si>
     <t>1 Hacker Way Menlo Park, CA 94025</t>
@@ -642,10 +648,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2">
@@ -653,10 +659,10 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3">
@@ -664,10 +670,10 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4">
@@ -675,10 +681,10 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -832,7 +838,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4">
@@ -840,7 +846,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5">
@@ -3855,13 +3861,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2">
@@ -3869,13 +3875,13 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3">
@@ -3883,13 +3889,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4">
@@ -3897,13 +3903,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -3930,10 +3936,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2">
@@ -3941,10 +3947,10 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3">
@@ -3952,10 +3958,10 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4">
@@ -3963,10 +3969,10 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -3992,7 +3998,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2">
@@ -4000,7 +4006,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3">
@@ -4008,7 +4014,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4">
@@ -4016,7 +4022,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -4042,10 +4048,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2">
@@ -4053,7 +4059,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C2" s="7">
         <v>60.0</v>
@@ -4064,7 +4070,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C3" s="7">
         <v>50.0</v>
@@ -4075,7 +4081,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C4" s="7">
         <v>60.0</v>
@@ -4106,13 +4112,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2">
@@ -4120,13 +4126,13 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3">
@@ -4134,13 +4140,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4">
@@ -4148,13 +4154,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
updated changes - 2022-07-04 19:28:45
</commit_message>
<xml_diff>
--- a/app/src/test/resources/Dataset.xlsx
+++ b/app/src/test/resources/Dataset.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="54">
   <si>
     <t>#</t>
   </si>
@@ -37,7 +37,10 @@
     <t>testPassword</t>
   </si>
   <si>
-    <t>test123</t>
+    <t>testUsername123</t>
+  </si>
+  <si>
+    <t>testPassword123</t>
   </si>
   <si>
     <t>test_123</t>
@@ -55,10 +58,10 @@
     <t>YONEX</t>
   </si>
   <si>
-    <t>ROADSTER</t>
-  </si>
-  <si>
-    <t>CONNECTOR</t>
+    <t>Roadster</t>
+  </si>
+  <si>
+    <t>Connector</t>
   </si>
   <si>
     <t>TC4_ProductNameToSearchFor</t>
@@ -67,9 +70,6 @@
     <t>Nike Mens Running Shoes</t>
   </si>
   <si>
-    <t>Roadster</t>
-  </si>
-  <si>
     <t>HandBag</t>
   </si>
   <si>
@@ -92,9 +92,6 @@
   </si>
   <si>
     <t>TEST ADDR LINES COUNT GREATER TH</t>
-  </si>
-  <si>
-    <t>Connector</t>
   </si>
   <si>
     <t>1 Hacker Way Menlo Park, CA 94025</t>
@@ -578,6 +575,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="2" max="2" width="24.75"/>
+    <col customWidth="1" min="3" max="3" width="18.5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -610,7 +608,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
@@ -618,10 +616,10 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -648,10 +646,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2">
@@ -670,10 +668,10 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4">
@@ -681,10 +679,10 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -703,6 +701,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="2" max="2" width="24.75"/>
+    <col customWidth="1" min="3" max="3" width="16.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -710,10 +709,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2">
@@ -735,7 +734,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
@@ -743,10 +742,10 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -772,7 +771,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2">
@@ -780,7 +779,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3">
@@ -788,7 +787,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
@@ -796,7 +795,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -822,7 +821,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2">
@@ -830,7 +829,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3">
@@ -838,7 +837,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
@@ -3906,10 +3905,10 @@
         <v>20</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -3936,10 +3935,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2">
@@ -3947,10 +3946,10 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="3">
@@ -3958,10 +3957,10 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4">
@@ -3969,10 +3968,10 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -3998,7 +3997,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2">
@@ -4006,7 +4005,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3">
@@ -4014,7 +4013,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4">
@@ -4022,7 +4021,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -4048,10 +4047,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2">
@@ -4070,7 +4069,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" s="7">
         <v>50.0</v>
@@ -4081,7 +4080,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4" s="7">
         <v>60.0</v>
@@ -4112,13 +4111,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="11" t="s">
         <v>40</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2">
@@ -4126,13 +4125,13 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="D2" s="12" t="s">
         <v>43</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="3">
@@ -4140,13 +4139,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="4">
@@ -4154,13 +4153,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
updated changes - 2022-07-04 19:28:47
</commit_message>
<xml_diff>
--- a/app/src/test/resources/Dataset.xlsx
+++ b/app/src/test/resources/Dataset.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="54">
   <si>
     <t>#</t>
   </si>
@@ -37,7 +37,10 @@
     <t>testPassword</t>
   </si>
   <si>
-    <t>test123</t>
+    <t>testUsername123</t>
+  </si>
+  <si>
+    <t>testPassword123</t>
   </si>
   <si>
     <t>test_123</t>
@@ -55,10 +58,10 @@
     <t>YONEX</t>
   </si>
   <si>
-    <t>ROADSTER</t>
-  </si>
-  <si>
-    <t>CONNECTOR</t>
+    <t>Roadster</t>
+  </si>
+  <si>
+    <t>Connector</t>
   </si>
   <si>
     <t>TC4_ProductNameToSearchFor</t>
@@ -67,9 +70,6 @@
     <t>Nike Mens Running Shoes</t>
   </si>
   <si>
-    <t>Roadster</t>
-  </si>
-  <si>
     <t>HandBag</t>
   </si>
   <si>
@@ -92,9 +92,6 @@
   </si>
   <si>
     <t>TEST ADDR LINES COUNT GREATER TH</t>
-  </si>
-  <si>
-    <t>Connector</t>
   </si>
   <si>
     <t>1 Hacker Way Menlo Park, CA 94025</t>
@@ -578,6 +575,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="2" max="2" width="24.75"/>
+    <col customWidth="1" min="3" max="3" width="18.5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -610,7 +608,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
@@ -618,10 +616,10 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -648,10 +646,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2">
@@ -670,10 +668,10 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4">
@@ -681,10 +679,10 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -703,6 +701,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="2" max="2" width="24.75"/>
+    <col customWidth="1" min="3" max="3" width="16.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -710,10 +709,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2">
@@ -735,7 +734,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
@@ -743,10 +742,10 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -772,7 +771,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2">
@@ -780,7 +779,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3">
@@ -788,7 +787,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
@@ -796,7 +795,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -822,7 +821,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2">
@@ -830,7 +829,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3">
@@ -838,7 +837,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
@@ -3906,10 +3905,10 @@
         <v>20</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -3936,10 +3935,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2">
@@ -3947,10 +3946,10 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="3">
@@ -3958,10 +3957,10 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4">
@@ -3969,10 +3968,10 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -3998,7 +3997,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2">
@@ -4006,7 +4005,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3">
@@ -4014,7 +4013,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4">
@@ -4022,7 +4021,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -4048,10 +4047,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2">
@@ -4070,7 +4069,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" s="7">
         <v>50.0</v>
@@ -4081,7 +4080,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4" s="7">
         <v>60.0</v>
@@ -4112,13 +4111,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="11" t="s">
         <v>40</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2">
@@ -4126,13 +4125,13 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="D2" s="12" t="s">
         <v>43</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="3">
@@ -4140,13 +4139,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="4">
@@ -4154,13 +4153,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
updated changes - 2022-07-04 19:28:50
</commit_message>
<xml_diff>
--- a/app/src/test/resources/Dataset.xlsx
+++ b/app/src/test/resources/Dataset.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="54">
   <si>
     <t>#</t>
   </si>
@@ -37,7 +37,10 @@
     <t>testPassword</t>
   </si>
   <si>
-    <t>test123</t>
+    <t>testUsername123</t>
+  </si>
+  <si>
+    <t>testPassword123</t>
   </si>
   <si>
     <t>test_123</t>
@@ -55,10 +58,10 @@
     <t>YONEX</t>
   </si>
   <si>
-    <t>ROADSTER</t>
-  </si>
-  <si>
-    <t>CONNECTOR</t>
+    <t>Roadster</t>
+  </si>
+  <si>
+    <t>Connector</t>
   </si>
   <si>
     <t>TC4_ProductNameToSearchFor</t>
@@ -67,9 +70,6 @@
     <t>Nike Mens Running Shoes</t>
   </si>
   <si>
-    <t>Roadster</t>
-  </si>
-  <si>
     <t>HandBag</t>
   </si>
   <si>
@@ -92,9 +92,6 @@
   </si>
   <si>
     <t>TEST ADDR LINES COUNT GREATER TH</t>
-  </si>
-  <si>
-    <t>Connector</t>
   </si>
   <si>
     <t>1 Hacker Way Menlo Park, CA 94025</t>
@@ -578,6 +575,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="2" max="2" width="24.75"/>
+    <col customWidth="1" min="3" max="3" width="18.5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -610,7 +608,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
@@ -618,10 +616,10 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -648,10 +646,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2">
@@ -670,10 +668,10 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4">
@@ -681,10 +679,10 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -703,6 +701,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="2" max="2" width="24.75"/>
+    <col customWidth="1" min="3" max="3" width="16.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -710,10 +709,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2">
@@ -735,7 +734,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
@@ -743,10 +742,10 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -772,7 +771,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2">
@@ -780,7 +779,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3">
@@ -788,7 +787,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
@@ -796,7 +795,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -822,7 +821,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2">
@@ -830,7 +829,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3">
@@ -838,7 +837,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
@@ -3906,10 +3905,10 @@
         <v>20</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -3936,10 +3935,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2">
@@ -3947,10 +3946,10 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="3">
@@ -3958,10 +3957,10 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4">
@@ -3969,10 +3968,10 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -3998,7 +3997,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2">
@@ -4006,7 +4005,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3">
@@ -4014,7 +4013,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4">
@@ -4022,7 +4021,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -4048,10 +4047,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2">
@@ -4070,7 +4069,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" s="7">
         <v>50.0</v>
@@ -4081,7 +4080,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4" s="7">
         <v>60.0</v>
@@ -4112,13 +4111,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="11" t="s">
         <v>40</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2">
@@ -4126,13 +4125,13 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="D2" s="12" t="s">
         <v>43</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="3">
@@ -4140,13 +4139,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="4">
@@ -4154,13 +4153,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
updated changes - 2022-07-04 19:28:53
</commit_message>
<xml_diff>
--- a/app/src/test/resources/Dataset.xlsx
+++ b/app/src/test/resources/Dataset.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="54">
   <si>
     <t>#</t>
   </si>
@@ -37,7 +37,10 @@
     <t>testPassword</t>
   </si>
   <si>
-    <t>test123</t>
+    <t>testUsername123</t>
+  </si>
+  <si>
+    <t>testPassword123</t>
   </si>
   <si>
     <t>test_123</t>
@@ -55,10 +58,10 @@
     <t>YONEX</t>
   </si>
   <si>
-    <t>ROADSTER</t>
-  </si>
-  <si>
-    <t>CONNECTOR</t>
+    <t>Roadster</t>
+  </si>
+  <si>
+    <t>Connector</t>
   </si>
   <si>
     <t>TC4_ProductNameToSearchFor</t>
@@ -67,9 +70,6 @@
     <t>Nike Mens Running Shoes</t>
   </si>
   <si>
-    <t>Roadster</t>
-  </si>
-  <si>
     <t>HandBag</t>
   </si>
   <si>
@@ -92,9 +92,6 @@
   </si>
   <si>
     <t>TEST ADDR LINES COUNT GREATER TH</t>
-  </si>
-  <si>
-    <t>Connector</t>
   </si>
   <si>
     <t>1 Hacker Way Menlo Park, CA 94025</t>
@@ -578,6 +575,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="2" max="2" width="24.75"/>
+    <col customWidth="1" min="3" max="3" width="18.5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -610,7 +608,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
@@ -618,10 +616,10 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -648,10 +646,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2">
@@ -670,10 +668,10 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4">
@@ -681,10 +679,10 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -703,6 +701,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="2" max="2" width="24.75"/>
+    <col customWidth="1" min="3" max="3" width="16.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -710,10 +709,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2">
@@ -735,7 +734,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
@@ -743,10 +742,10 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -772,7 +771,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2">
@@ -780,7 +779,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3">
@@ -788,7 +787,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
@@ -796,7 +795,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -822,7 +821,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2">
@@ -830,7 +829,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3">
@@ -838,7 +837,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
@@ -3906,10 +3905,10 @@
         <v>20</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -3936,10 +3935,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2">
@@ -3947,10 +3946,10 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="3">
@@ -3958,10 +3957,10 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4">
@@ -3969,10 +3968,10 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -3998,7 +3997,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2">
@@ -4006,7 +4005,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3">
@@ -4014,7 +4013,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4">
@@ -4022,7 +4021,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -4048,10 +4047,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2">
@@ -4070,7 +4069,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" s="7">
         <v>50.0</v>
@@ -4081,7 +4080,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4" s="7">
         <v>60.0</v>
@@ -4112,13 +4111,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="11" t="s">
         <v>40</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2">
@@ -4126,13 +4125,13 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="D2" s="12" t="s">
         <v>43</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="3">
@@ -4140,13 +4139,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="4">
@@ -4154,13 +4153,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
updated changes - 2022-07-04 19:28:57
</commit_message>
<xml_diff>
--- a/app/src/test/resources/Dataset.xlsx
+++ b/app/src/test/resources/Dataset.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="54">
   <si>
     <t>#</t>
   </si>
@@ -37,7 +37,10 @@
     <t>testPassword</t>
   </si>
   <si>
-    <t>test123</t>
+    <t>testUsername123</t>
+  </si>
+  <si>
+    <t>testPassword123</t>
   </si>
   <si>
     <t>test_123</t>
@@ -55,10 +58,10 @@
     <t>YONEX</t>
   </si>
   <si>
-    <t>ROADSTER</t>
-  </si>
-  <si>
-    <t>CONNECTOR</t>
+    <t>Roadster</t>
+  </si>
+  <si>
+    <t>Connector</t>
   </si>
   <si>
     <t>TC4_ProductNameToSearchFor</t>
@@ -67,9 +70,6 @@
     <t>Nike Mens Running Shoes</t>
   </si>
   <si>
-    <t>Roadster</t>
-  </si>
-  <si>
     <t>HandBag</t>
   </si>
   <si>
@@ -92,9 +92,6 @@
   </si>
   <si>
     <t>TEST ADDR LINES COUNT GREATER TH</t>
-  </si>
-  <si>
-    <t>Connector</t>
   </si>
   <si>
     <t>1 Hacker Way Menlo Park, CA 94025</t>
@@ -578,6 +575,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="2" max="2" width="24.75"/>
+    <col customWidth="1" min="3" max="3" width="18.5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -610,7 +608,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
@@ -618,10 +616,10 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -648,10 +646,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2">
@@ -670,10 +668,10 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4">
@@ -681,10 +679,10 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -703,6 +701,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="2" max="2" width="24.75"/>
+    <col customWidth="1" min="3" max="3" width="16.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -710,10 +709,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2">
@@ -735,7 +734,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
@@ -743,10 +742,10 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -772,7 +771,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2">
@@ -780,7 +779,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3">
@@ -788,7 +787,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
@@ -796,7 +795,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -822,7 +821,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2">
@@ -830,7 +829,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3">
@@ -838,7 +837,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
@@ -3906,10 +3905,10 @@
         <v>20</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -3936,10 +3935,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2">
@@ -3947,10 +3946,10 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="3">
@@ -3958,10 +3957,10 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4">
@@ -3969,10 +3968,10 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -3998,7 +3997,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2">
@@ -4006,7 +4005,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3">
@@ -4014,7 +4013,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4">
@@ -4022,7 +4021,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -4048,10 +4047,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2">
@@ -4070,7 +4069,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" s="7">
         <v>50.0</v>
@@ -4081,7 +4080,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4" s="7">
         <v>60.0</v>
@@ -4112,13 +4111,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="11" t="s">
         <v>40</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2">
@@ -4126,13 +4125,13 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="D2" s="12" t="s">
         <v>43</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="3">
@@ -4140,13 +4139,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="4">
@@ -4154,13 +4153,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="5">

</xml_diff>